<commit_message>
tg: update sch/sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/2024/tg_sch_sth_ia_202404_2_kk.xlsx
+++ b/SCH-STH/Impact assessments/Togo/2024/tg_sch_sth_ia_202404_2_kk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Togo\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B5E8AB-AC75-411A-A69C-F66B19705F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43A629-DFA0-4712-94D1-E991D4736194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1183,7 +1183,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1433,7 +1433,7 @@
     </row>
     <row r="11" spans="1:13" s="32" customFormat="1" ht="31.5">
       <c r="A11" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
to: update list som forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Togo/2024/tg_sch_sth_ia_202404_2_kk.xlsx
+++ b/SCH-STH/Impact assessments/Togo/2024/tg_sch_sth_ia_202404_2_kk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Togo\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43A629-DFA0-4712-94D1-E991D4736194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C437E0-71B9-42D8-9955-84E64B557FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -350,12 +350,6 @@
     <t>if (${C2} = 1,'',substring-after(${C1},${k_barcodeid}))</t>
   </si>
   <si>
-    <t>not(selected(${C3}, ${k_barcodeid}))</t>
-  </si>
-  <si>
-    <t>Ce QR Code est déjà utilisé</t>
-  </si>
-  <si>
     <t>end repeat</t>
   </si>
   <si>
@@ -491,18 +485,9 @@
     <t xml:space="preserve">N DATO Kossi </t>
   </si>
   <si>
-    <t>tg_sch_sth_ia_202404_2_kk_v3</t>
-  </si>
-  <si>
-    <t>(2024 Avr) - 2. SCH/STH - Kato Katz V3</t>
-  </si>
-  <si>
     <t>repeat_count</t>
   </si>
   <si>
-    <t>tg_sch_sth_k_2404_v3</t>
-  </si>
-  <si>
     <t>k_nb_children</t>
   </si>
   <si>
@@ -510,6 +495,23 @@
   </si>
   <si>
     <t>${k_nb_children}</t>
+  </si>
+  <si>
+    <t>not(selected(${C3}, ${k_barcodeid})) and 
+regex(.,'^(BLI|AGO|ASS|BIN|DAN|DOU|KER|KOZ|AVE|BAS|LAC|VOG|YOT|ZIO)_\d{4}$') and 
+(substr(${k_district} , 0, 3) = substr(., 0, 3) or substr(${k_district} , 0, 3) = 'VO')</t>
+  </si>
+  <si>
+    <t>Ce QR Code n'appartient pas à ce district ou vous l'avez déjà utiliser</t>
+  </si>
+  <si>
+    <t>(2024 Avr) - 2. SCH/STH - Kato Katz V3.1</t>
+  </si>
+  <si>
+    <t>tg_sch_sth_ia_202404_2_kk_v3_1</t>
+  </si>
+  <si>
+    <t>tg_sch_sth_k_2404_v3_1</t>
   </si>
 </sst>
 </file>
@@ -1183,7 +1185,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1193,7 +1195,7 @@
     <col min="3" max="3" width="47.5" style="39" customWidth="1"/>
     <col min="4" max="4" width="47.375" style="19" customWidth="1"/>
     <col min="5" max="5" width="12.625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="16.875" style="39" customWidth="1"/>
+    <col min="6" max="6" width="31.875" style="39" customWidth="1"/>
     <col min="7" max="7" width="29.5" style="19" customWidth="1"/>
     <col min="8" max="8" width="22" style="19" customWidth="1"/>
     <col min="9" max="9" width="12.625" style="19" customWidth="1"/>
@@ -1241,21 +1243,21 @@
         <v>11</v>
       </c>
       <c r="M1" s="51" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="18" customFormat="1">
       <c r="A2" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E2" s="50"/>
       <c r="F2" s="8"/>
@@ -1339,10 +1341,10 @@
         <v>22</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="J6" s="54" t="s">
         <v>13</v>
@@ -1368,12 +1370,12 @@
       <c r="K7" s="22"/>
       <c r="L7" s="30"/>
     </row>
-    <row r="8" spans="1:13" s="18" customFormat="1">
+    <row r="8" spans="1:13" s="18" customFormat="1" ht="31.5">
       <c r="A8" s="41" t="s">
         <v>89</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>90</v>
@@ -1388,7 +1390,7 @@
       <c r="K8" s="41"/>
       <c r="L8" s="41"/>
       <c r="M8" s="18" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="18" customFormat="1">
@@ -1431,7 +1433,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="29"/>
     </row>
-    <row r="11" spans="1:13" s="32" customFormat="1" ht="31.5">
+    <row r="11" spans="1:13" s="32" customFormat="1" ht="126">
       <c r="A11" s="20" t="s">
         <v>19</v>
       </c>
@@ -1444,10 +1446,10 @@
       <c r="D11" s="21"/>
       <c r="E11" s="20"/>
       <c r="F11" s="22" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>97</v>
+        <v>146</v>
       </c>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
@@ -1935,7 +1937,7 @@
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B34" s="43"/>
       <c r="C34" s="44"/>
@@ -2061,10 +2063,10 @@
         <v>53</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="14"/>
@@ -2075,10 +2077,10 @@
         <v>53</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="14"/>
@@ -2089,10 +2091,10 @@
         <v>53</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="14"/>
@@ -2103,10 +2105,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="14"/>
@@ -2117,10 +2119,10 @@
         <v>53</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="14"/>
@@ -2131,10 +2133,10 @@
         <v>53</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="14"/>
@@ -2145,10 +2147,10 @@
         <v>53</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="14"/>
@@ -2159,10 +2161,10 @@
         <v>53</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="14"/>
@@ -2173,10 +2175,10 @@
         <v>53</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="14"/>
@@ -2187,10 +2189,10 @@
         <v>53</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="14"/>
@@ -2201,10 +2203,10 @@
         <v>53</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="14"/>
@@ -2215,10 +2217,10 @@
         <v>53</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="14"/>
@@ -2229,10 +2231,10 @@
         <v>53</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="14"/>
@@ -2243,10 +2245,10 @@
         <v>53</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="14"/>
@@ -2257,10 +2259,10 @@
         <v>53</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="14"/>
@@ -2271,10 +2273,10 @@
         <v>53</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="14"/>
@@ -2285,10 +2287,10 @@
         <v>53</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="14"/>
@@ -2299,10 +2301,10 @@
         <v>53</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="14"/>
@@ -2327,10 +2329,10 @@
         <v>53</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="14"/>
@@ -2341,10 +2343,10 @@
         <v>53</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="14"/>
@@ -2355,10 +2357,10 @@
         <v>53</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="14"/>
@@ -2369,10 +2371,10 @@
         <v>53</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="14"/>
@@ -2383,10 +2385,10 @@
         <v>53</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="14"/>
@@ -2397,10 +2399,10 @@
         <v>53</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="14"/>
@@ -2411,10 +2413,10 @@
         <v>53</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="14"/>
@@ -2425,10 +2427,10 @@
         <v>53</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="14"/>
@@ -2439,10 +2441,10 @@
         <v>53</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="14"/>
@@ -2453,10 +2455,10 @@
         <v>53</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="14"/>
@@ -2467,10 +2469,10 @@
         <v>53</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="14"/>
@@ -2481,10 +2483,10 @@
         <v>53</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="14"/>
@@ -2495,10 +2497,10 @@
         <v>53</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="14"/>
@@ -2509,10 +2511,10 @@
         <v>53</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="14"/>
@@ -2523,10 +2525,10 @@
         <v>53</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="14"/>
@@ -2537,10 +2539,10 @@
         <v>53</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="14"/>
@@ -2551,10 +2553,10 @@
         <v>53</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="14"/>
@@ -2565,10 +2567,10 @@
         <v>53</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="14"/>
@@ -2579,10 +2581,10 @@
         <v>53</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="14"/>
@@ -2593,10 +2595,10 @@
         <v>53</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="14"/>
@@ -2621,10 +2623,10 @@
         <v>53</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="14"/>
@@ -3737,7 +3739,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3762,10 +3764,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="18" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>

</xml_diff>